<commit_message>
nova rodada 1 a 9
</commit_message>
<xml_diff>
--- a/backup_1_9/plotQtdAlternatives.xlsx
+++ b/backup_1_9/plotQtdAlternatives.xlsx
@@ -639,58 +639,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>0.87333333333333296</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.89523809523809506</c:v>
+                  <c:v>0.92380952380952297</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.74404761904761896</c:v>
+                  <c:v>0.766156462585034</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.871913589564416</c:v>
+                  <c:v>0.865274395425222</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.83568437030702003</c:v>
+                  <c:v>0.83731617402802405</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.88414902996042</c:v>
+                  <c:v>0.88213455732289003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.90323468485580904</c:v>
+                  <c:v>0.900917054311282</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.87694625063046105</c:v>
+                  <c:v>0.87597908913698297</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.93794834756541301</c:v>
+                  <c:v>0.93864199259050796</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.94488139360968004</c:v>
+                  <c:v>0.94617769342626301</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.95368371763390103</c:v>
+                  <c:v>0.95423071935802595</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.93704044117647001</c:v>
+                  <c:v>0.93777573529411695</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.97448096885813096</c:v>
+                  <c:v>0.97390426758938797</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.76879039704524399</c:v>
+                  <c:v>0.76934441366574302</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.89307330195080903</c:v>
+                  <c:v>0.88942118937537795</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.92270819936510295</c:v>
+                  <c:v>0.92143959548951304</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.98809932978174897</c:v>
+                  <c:v>0.98792747894827304</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.928192351320693</c:v>
+                  <c:v>0.92871900826446296</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -784,58 +784,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>0.81111111111111101</c:v>
+                  <c:v>0.97777777777777697</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.98148148148148096</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.75595238095238004</c:v>
+                  <c:v>0.83333333333333304</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.83613782051282004</c:v>
+                  <c:v>0.86538461538461497</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.763348148148148</c:v>
+                  <c:v>0.89688888888888796</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.82012903225806399</c:v>
+                  <c:v>0.88593548387096699</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.88606060606060599</c:v>
+                  <c:v>0.89545454545454495</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.72322530864197498</c:v>
+                  <c:v>0.81944444444444398</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.77343668236525298</c:v>
+                  <c:v>0.95604395604395598</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.908193634596695</c:v>
+                  <c:v>0.88775510204081598</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.85109523809523802</c:v>
+                  <c:v>0.97</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.88496093749999905</c:v>
+                  <c:v>0.9375</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.86362952588442699</c:v>
+                  <c:v>0.99346405228758095</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.64253968253968197</c:v>
+                  <c:v>0.78947368421052599</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.81355555555555503</c:v>
+                  <c:v>0.875</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.76772393071094303</c:v>
+                  <c:v>0.939393939393939</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.92868200639939702</c:v>
+                  <c:v>0.98913043478260798</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.75722181698510704</c:v>
+                  <c:v>0.92156862745098</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -929,68 +929,68 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>0.93111934426067799</c:v>
+                  <c:v>0.93282235593109597</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.99647521864725797</c:v>
+                  <c:v>0.99817812147912899</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.90220350797422699</c:v>
+                  <c:v>0.91601796075007402</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.95393688176893898</c:v>
+                  <c:v>0.955497776164278</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.90187972150623097</c:v>
+                  <c:v>0.89892634517564296</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.93428774088857502</c:v>
+                  <c:v>0.93257692002981196</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.96611596082708195</c:v>
+                  <c:v>0.96702327112215203</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.87169876401981405</c:v>
+                  <c:v>0.85686974580470099</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.82259924189419298</c:v>
+                  <c:v>0.82311710765713197</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.97985875488684604</c:v>
+                  <c:v>0.97991904493109905</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.93437459098126596</c:v>
+                  <c:v>0.92863837335586996</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.99158615393371297</c:v>
+                  <c:v>0.99057939970540398</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.95071068150022697</c:v>
+                  <c:v>0.95134008585220597</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.85121832575856504</c:v>
+                  <c:v>0.85108623572032904</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.97853867927567895</c:v>
+                  <c:v>0.97870349811620305</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.92659178732542002</c:v>
+                  <c:v>0.92933967525314698</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.99311914164287496</c:v>
+                  <c:v>0.99425083525449298</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.87198133600296202</c:v>
+                  <c:v>0.87178696397460698</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="47289088"/>
-        <c:axId val="47290624"/>
+        <c:axId val="48861184"/>
+        <c:axId val="48862720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="47289088"/>
+        <c:axId val="48861184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="3"/>
@@ -998,21 +998,21 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47290624"/>
+        <c:crossAx val="48862720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="47290624"/>
+        <c:axId val="48862720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="0.6000000000000002"/>
+          <c:min val="0.60000000000000031"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47289088"/>
+        <c:crossAx val="48861184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1025,7 +1025,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000014" footer="0.31496062000000014"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000025" footer="0.31496062000000025"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1126,80 +1126,80 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>2.53713094342988E-2</c:v>
+                  <c:v>2.6824275480807801E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.9408994506949299E-2</c:v>
+                  <c:v>2.67132859574284E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.88457123087421E-2</c:v>
+                  <c:v>2.7099834608234102E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.0019547881525501E-2</c:v>
+                  <c:v>2.31425664552002E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.0136482849471199E-2</c:v>
+                  <c:v>2.3495008000735399E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.43003974985117E-2</c:v>
+                  <c:v>1.52676533670386E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.18473741967397E-2</c:v>
+                  <c:v>1.2466162868590199E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.55043635492594E-2</c:v>
+                  <c:v>2.5521178840814399E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.6451825624302301E-2</c:v>
+                  <c:v>1.74735945613936E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.3710710275535701E-2</c:v>
+                  <c:v>2.3688014419403901E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.3539959846649506E-3</c:v>
+                  <c:v>9.4252068614306406E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.1934534497139699E-2</c:v>
+                  <c:v>1.18529249979586E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.60579708115325E-3</c:v>
+                  <c:v>6.5932661005393897E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.74919100253345E-2</c:v>
+                  <c:v>2.7530766094265E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.23697994630997E-2</c:v>
+                  <c:v>1.2373290899468099E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7.89462553825079E-3</c:v>
+                  <c:v>7.9539808780451204E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.80267654095132E-3</c:v>
+                  <c:v>1.7989952277666201E-3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.0708076293301601E-2</c:v>
+                  <c:v>2.0704068522324499E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="47307008"/>
-        <c:axId val="47325184"/>
+        <c:axId val="48965120"/>
+        <c:axId val="48966656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="47307008"/>
+        <c:axId val="48965120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47325184"/>
+        <c:crossAx val="48966656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="47325184"/>
+        <c:axId val="48966656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1207,7 +1207,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47307008"/>
+        <c:crossAx val="48965120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1220,7 +1220,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000025" footer="0.31496062000000025"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000036" footer="0.31496062000000036"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1258,10 +1258,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Qtd Alternativas NO'!$A$1:$A$15</c:f>
+              <c:f>'Qtd Alternativas NO'!$A$1:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -1300,66 +1300,54 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Qtd Alternativas NO'!$D$1:$D$15</c:f>
+              <c:f>'Qtd Alternativas NO'!$D$1:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>0.87333333333333296</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.89523809523809506</c:v>
+                  <c:v>0.92380952380952297</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.871913589564416</c:v>
+                  <c:v>0.865274395425222</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.83568437030702003</c:v>
+                  <c:v>0.83731617402802405</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.88414902996042</c:v>
+                  <c:v>0.88213455732289003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.90323468485580904</c:v>
+                  <c:v>0.900917054311282</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.87694625063046105</c:v>
+                  <c:v>0.87597908913698297</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.93794834756541301</c:v>
+                  <c:v>0.93864199259050796</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.94488139360968004</c:v>
+                  <c:v>0.94617769342626301</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.95368371763390103</c:v>
+                  <c:v>0.95423071935802595</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.93704044117647001</c:v>
+                  <c:v>0.93777573529411695</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.97448096885813096</c:v>
+                  <c:v>0.97390426758938797</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.89307330195080903</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.92270819936510295</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.98809932978174897</c:v>
+                  <c:v>0.88942118937537795</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1389,10 +1377,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Qtd Alternativas NO'!$A$1:$A$15</c:f>
+              <c:f>'Qtd Alternativas NO'!$A$1:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -1431,66 +1419,54 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Qtd Alternativas NO'!$F$1:$F$15</c:f>
+              <c:f>'Qtd Alternativas NO'!$F$1:$F$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>0.81111111111111101</c:v>
+                  <c:v>0.97777777777777697</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.98148148148148096</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.83613782051282004</c:v>
+                  <c:v>0.86538461538461497</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.763348148148148</c:v>
+                  <c:v>0.89688888888888796</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.82012903225806399</c:v>
+                  <c:v>0.88593548387096699</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.88606060606060599</c:v>
+                  <c:v>0.89545454545454495</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.72322530864197498</c:v>
+                  <c:v>0.81944444444444398</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.77343668236525298</c:v>
+                  <c:v>0.95604395604395598</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.908193634596695</c:v>
+                  <c:v>0.88775510204081598</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.85109523809523802</c:v>
+                  <c:v>0.97</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.88496093749999905</c:v>
+                  <c:v>0.9375</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.86362952588442699</c:v>
+                  <c:v>0.99346405228758095</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.81355555555555503</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.76772393071094303</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.92868200639939702</c:v>
+                  <c:v>0.875</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1520,10 +1496,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Qtd Alternativas NO'!$A$1:$A$15</c:f>
+              <c:f>'Qtd Alternativas NO'!$A$1:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -1562,97 +1538,85 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Qtd Alternativas NO'!$H$1:$H$15</c:f>
+              <c:f>'Qtd Alternativas NO'!$H$1:$H$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>0.93111934426067799</c:v>
+                  <c:v>0.93282235593109597</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.99647521864725797</c:v>
+                  <c:v>0.99817812147912899</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.95393688176893898</c:v>
+                  <c:v>0.955497776164278</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.90187972150623097</c:v>
+                  <c:v>0.89892634517564296</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.93428774088857502</c:v>
+                  <c:v>0.93257692002981196</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.96611596082708195</c:v>
+                  <c:v>0.96702327112215203</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.87169876401981405</c:v>
+                  <c:v>0.85686974580470099</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.82259924189419298</c:v>
+                  <c:v>0.82311710765713197</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.97985875488684604</c:v>
+                  <c:v>0.97991904493109905</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.93437459098126596</c:v>
+                  <c:v>0.92863837335586996</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.99158615393371297</c:v>
+                  <c:v>0.99057939970540398</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.95071068150022697</c:v>
+                  <c:v>0.95134008585220597</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.97853867927567895</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.92659178732542002</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.99311914164287496</c:v>
+                  <c:v>0.97870349811620305</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="47214592"/>
-        <c:axId val="47216128"/>
+        <c:axId val="48925696"/>
+        <c:axId val="48939776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="47214592"/>
+        <c:axId val="48925696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47216128"/>
+        <c:crossAx val="48939776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="47216128"/>
+        <c:axId val="48939776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="0.60000000000000031"/>
+          <c:min val="0.60000000000000042"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47214592"/>
+        <c:crossAx val="48925696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.05"/>
@@ -1666,7 +1630,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000036" footer="0.31496062000000036"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000041" footer="0.31496062000000041"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1699,10 +1663,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Qtd Alternativas NO'!$A$1:$A$15</c:f>
+              <c:f>'Qtd Alternativas NO'!$A$1:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -1741,88 +1705,76 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Qtd Alternativas NO'!$B$1:$B$15</c:f>
+              <c:f>'Qtd Alternativas NO'!$B$1:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>2.53713094342988E-2</c:v>
+                  <c:v>2.6824275480807801E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.9408994506949299E-2</c:v>
+                  <c:v>2.67132859574284E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0019547881525501E-2</c:v>
+                  <c:v>2.31425664552002E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.0136482849471199E-2</c:v>
+                  <c:v>2.3495008000735399E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.43003974985117E-2</c:v>
+                  <c:v>1.52676533670386E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.18473741967397E-2</c:v>
+                  <c:v>1.2466162868590199E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.55043635492594E-2</c:v>
+                  <c:v>2.5521178840814399E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.6451825624302301E-2</c:v>
+                  <c:v>1.74735945613936E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.3710710275535701E-2</c:v>
+                  <c:v>2.3688014419403901E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.3539959846649506E-3</c:v>
+                  <c:v>9.4252068614306406E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.1934534497139699E-2</c:v>
+                  <c:v>1.18529249979586E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.60579708115325E-3</c:v>
+                  <c:v>6.5932661005393897E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.23697994630997E-2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>7.89462553825079E-3</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.80267654095132E-3</c:v>
+                  <c:v>1.2373290899468099E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="47387776"/>
-        <c:axId val="47389312"/>
+        <c:axId val="49103232"/>
+        <c:axId val="49104768"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="47387776"/>
+        <c:axId val="49103232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47389312"/>
+        <c:crossAx val="49104768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="47389312"/>
+        <c:axId val="49104768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1830,7 +1782,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47387776"/>
+        <c:crossAx val="49103232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1843,7 +1795,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000008" footer="0.31496062000000008"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000014" footer="0.31496062000000014"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1920,13 +1872,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>85726</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1950,13 +1902,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>638175</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2267,7 +2219,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection sqref="A1:I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2286,28 +2238,28 @@
         <v>5</v>
       </c>
       <c r="B1">
-        <v>2.53713094342988E-2</v>
+        <v>2.6824275480807801E-2</v>
       </c>
       <c r="C1">
-        <v>1.7375272644192301E-2</v>
+        <v>1.5764321153293199E-2</v>
       </c>
       <c r="D1">
-        <v>0.87333333333333296</v>
+        <v>0.9</v>
       </c>
       <c r="E1">
-        <v>0.122202018532155</v>
+        <v>0.13999999999999899</v>
       </c>
       <c r="F1">
-        <v>0.81111111111111101</v>
+        <v>0.97777777777777697</v>
       </c>
       <c r="G1">
-        <v>0.24570382652773301</v>
+        <v>3.8490017945975098E-2</v>
       </c>
       <c r="H1">
-        <v>0.93111934426067799</v>
+        <v>0.93282235593109597</v>
       </c>
       <c r="I1">
-        <v>0.109970224219978</v>
+        <v>0.111365836959813</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -2315,25 +2267,25 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>2.9408994506949299E-2</v>
+        <v>2.67132859574284E-2</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0.89523809523809506</v>
+        <v>0.92380952380952297</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0.98148148148148096</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>0.99647521864725797</v>
+        <v>0.99817812147912899</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -2344,28 +2296,28 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>2.88457123087421E-2</v>
+        <v>2.7099834608234102E-2</v>
       </c>
       <c r="C3">
-        <v>1.71718617233073E-2</v>
+        <v>1.24712524973762E-2</v>
       </c>
       <c r="D3">
-        <v>0.74404761904761896</v>
+        <v>0.766156462585034</v>
       </c>
       <c r="E3">
-        <v>0.244097686205625</v>
+        <v>0.21453864243764201</v>
       </c>
       <c r="F3">
-        <v>0.75595238095238004</v>
+        <v>0.83333333333333304</v>
       </c>
       <c r="G3">
-        <v>0.20094025014163799</v>
+        <v>0.107538950387011</v>
       </c>
       <c r="H3">
-        <v>0.90220350797422699</v>
+        <v>0.91601796075007402</v>
       </c>
       <c r="I3">
-        <v>9.9929471934676703E-2</v>
+        <v>7.3717094922444396E-2</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -2373,28 +2325,28 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>2.0019547881525501E-2</v>
+        <v>2.31425664552002E-2</v>
       </c>
       <c r="C4">
-        <v>1.2512717333423001E-2</v>
+        <v>1.48067928919965E-2</v>
       </c>
       <c r="D4">
-        <v>0.871913589564416</v>
+        <v>0.865274395425222</v>
       </c>
       <c r="E4">
-        <v>0.131457001209317</v>
+        <v>0.13989032401443099</v>
       </c>
       <c r="F4">
-        <v>0.83613782051282004</v>
+        <v>0.86538461538461497</v>
       </c>
       <c r="G4">
-        <v>0.13032746953567201</v>
+        <v>0.125898215145899</v>
       </c>
       <c r="H4">
-        <v>0.95393688176893898</v>
+        <v>0.955497776164278</v>
       </c>
       <c r="I4">
-        <v>4.9147590797853802E-2</v>
+        <v>4.7503973139513801E-2</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -2402,28 +2354,28 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>2.0136482849471199E-2</v>
+        <v>2.3495008000735399E-2</v>
       </c>
       <c r="C5">
-        <v>1.44457556041197E-2</v>
+        <v>1.5599641359644799E-2</v>
       </c>
       <c r="D5">
-        <v>0.83568437030702003</v>
+        <v>0.83731617402802405</v>
       </c>
       <c r="E5">
-        <v>0.16564227359021699</v>
+        <v>0.15930951969790899</v>
       </c>
       <c r="F5">
-        <v>0.763348148148148</v>
+        <v>0.89688888888888796</v>
       </c>
       <c r="G5">
-        <v>0.184342232078445</v>
+        <v>0.10018090632335799</v>
       </c>
       <c r="H5">
-        <v>0.90187972150623097</v>
+        <v>0.89892634517564296</v>
       </c>
       <c r="I5">
-        <v>0.11985644698003201</v>
+        <v>0.10877767414772201</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -2431,28 +2383,28 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>1.43003974985117E-2</v>
+        <v>1.52676533670386E-2</v>
       </c>
       <c r="C6">
-        <v>9.01065114810801E-3</v>
+        <v>1.0100009553653E-2</v>
       </c>
       <c r="D6">
-        <v>0.88414902996042</v>
+        <v>0.88213455732289003</v>
       </c>
       <c r="E6">
-        <v>0.123133644282738</v>
+        <v>0.12055886020038099</v>
       </c>
       <c r="F6">
-        <v>0.82012903225806399</v>
+        <v>0.88593548387096699</v>
       </c>
       <c r="G6">
-        <v>0.133496893117409</v>
+        <v>0.109809142418529</v>
       </c>
       <c r="H6">
-        <v>0.93428774088857502</v>
+        <v>0.93257692002981196</v>
       </c>
       <c r="I6">
-        <v>7.7273945438372793E-2</v>
+        <v>7.4727421422603996E-2</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -2460,28 +2412,28 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>1.18473741967397E-2</v>
+        <v>1.2466162868590199E-2</v>
       </c>
       <c r="C7">
-        <v>5.4360729953337496E-3</v>
+        <v>5.3243719083130399E-3</v>
       </c>
       <c r="D7">
-        <v>0.90323468485580904</v>
+        <v>0.900917054311282</v>
       </c>
       <c r="E7">
-        <v>0.107781534508995</v>
+        <v>0.111169088979949</v>
       </c>
       <c r="F7">
-        <v>0.88606060606060599</v>
+        <v>0.89545454545454495</v>
       </c>
       <c r="G7">
-        <v>9.3037026435947301E-2</v>
+        <v>9.7528377981921294E-2</v>
       </c>
       <c r="H7">
-        <v>0.96611596082708195</v>
+        <v>0.96702327112215203</v>
       </c>
       <c r="I7">
-        <v>3.8001592007031897E-2</v>
+        <v>4.1124123150383697E-2</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -2489,28 +2441,28 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>2.55043635492594E-2</v>
+        <v>2.5521178840814399E-2</v>
       </c>
       <c r="C8">
-        <v>9.5578098285571504E-3</v>
+        <v>9.3684982629107204E-3</v>
       </c>
       <c r="D8">
-        <v>0.87694625063046105</v>
+        <v>0.87597908913698297</v>
       </c>
       <c r="E8">
-        <v>6.2404683853617499E-2</v>
+        <v>6.3668976897568993E-2</v>
       </c>
       <c r="F8">
-        <v>0.72322530864197498</v>
+        <v>0.81944444444444398</v>
       </c>
       <c r="G8">
-        <v>0.156445236963276</v>
+        <v>1.38888888888889E-2</v>
       </c>
       <c r="H8">
-        <v>0.87169876401981405</v>
+        <v>0.85686974580470099</v>
       </c>
       <c r="I8">
-        <v>0.104001109554501</v>
+        <v>0.11280351961559899</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -2518,28 +2470,28 @@
         <v>13</v>
       </c>
       <c r="B9">
-        <v>1.6451825624302301E-2</v>
+        <v>1.74735945613936E-2</v>
       </c>
       <c r="C9">
-        <v>1.25178536920993E-2</v>
+        <v>1.3769354769872099E-2</v>
       </c>
       <c r="D9">
-        <v>0.93794834756541301</v>
+        <v>0.93864199259050796</v>
       </c>
       <c r="E9">
-        <v>7.2185737160212801E-2</v>
+        <v>7.2386666072416894E-2</v>
       </c>
       <c r="F9">
-        <v>0.77343668236525298</v>
+        <v>0.95604395604395598</v>
       </c>
       <c r="G9">
-        <v>0.169953076549888</v>
+        <v>1.7944979800609301E-2</v>
       </c>
       <c r="H9">
-        <v>0.82259924189419298</v>
+        <v>0.82311710765713197</v>
       </c>
       <c r="I9">
-        <v>0.15784888156597801</v>
+        <v>0.158368480855583</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -2547,28 +2499,28 @@
         <v>14</v>
       </c>
       <c r="B10">
-        <v>2.3710710275535701E-2</v>
+        <v>2.3688014419403901E-2</v>
       </c>
       <c r="C10">
-        <v>3.0339835540402999E-2</v>
+        <v>3.0401135640758199E-2</v>
       </c>
       <c r="D10">
-        <v>0.94488139360968004</v>
+        <v>0.94617769342626301</v>
       </c>
       <c r="E10">
-        <v>2.6375727759949601E-2</v>
+        <v>2.5453420067175901E-2</v>
       </c>
       <c r="F10">
-        <v>0.908193634596695</v>
+        <v>0.88775510204081598</v>
       </c>
       <c r="G10">
-        <v>9.0097593455366998E-2</v>
+        <v>2.6346825484404202E-2</v>
       </c>
       <c r="H10">
-        <v>0.97985875488684604</v>
+        <v>0.97991904493109905</v>
       </c>
       <c r="I10">
-        <v>3.3038928126666797E-2</v>
+        <v>3.3054929158388202E-2</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -2576,28 +2528,28 @@
         <v>15</v>
       </c>
       <c r="B11">
-        <v>9.3539959846649506E-3</v>
+        <v>9.4252068614306406E-3</v>
       </c>
       <c r="C11">
-        <v>6.8018027041726603E-3</v>
+        <v>6.9030166424523098E-3</v>
       </c>
       <c r="D11">
-        <v>0.95368371763390103</v>
+        <v>0.95423071935802595</v>
       </c>
       <c r="E11">
-        <v>4.6066818023423002E-2</v>
+        <v>4.5016071477029101E-2</v>
       </c>
       <c r="F11">
-        <v>0.85109523809523802</v>
+        <v>0.97</v>
       </c>
       <c r="G11">
-        <v>0.108601569420764</v>
+        <v>3.8459935864047702E-2</v>
       </c>
       <c r="H11">
-        <v>0.93437459098126596</v>
+        <v>0.92863837335586996</v>
       </c>
       <c r="I11">
-        <v>7.6102795407862606E-2</v>
+        <v>8.0020544207184297E-2</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -2605,28 +2557,28 @@
         <v>16</v>
       </c>
       <c r="B12">
-        <v>1.1934534497139699E-2</v>
+        <v>1.18529249979586E-2</v>
       </c>
       <c r="C12">
-        <v>4.0604974111013298E-3</v>
+        <v>4.0371560923254304E-3</v>
       </c>
       <c r="D12">
-        <v>0.93704044117647001</v>
+        <v>0.93777573529411695</v>
       </c>
       <c r="E12">
-        <v>2.6906452887061501E-2</v>
+        <v>2.92461444424581E-2</v>
       </c>
       <c r="F12">
-        <v>0.88496093749999905</v>
+        <v>0.9375</v>
       </c>
       <c r="G12">
-        <v>9.9173830545879194E-3</v>
+        <v>7.7339804192278594E-2</v>
       </c>
       <c r="H12">
-        <v>0.99158615393371297</v>
+        <v>0.99057939970540398</v>
       </c>
       <c r="I12">
-        <v>2.4966373300413201E-3</v>
+        <v>4.8441530992826397E-3</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -2634,25 +2586,25 @@
         <v>17</v>
       </c>
       <c r="B13">
-        <v>6.60579708115325E-3</v>
+        <v>6.5932661005393897E-3</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13">
-        <v>0.97448096885813096</v>
+        <v>0.97390426758938797</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="F13">
-        <v>0.86362952588442699</v>
+        <v>0.99346405228758095</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13">
-        <v>0.95071068150022697</v>
+        <v>0.95134008585220597</v>
       </c>
       <c r="I13">
         <v>0</v>
@@ -2663,25 +2615,25 @@
         <v>19</v>
       </c>
       <c r="B14">
-        <v>2.74919100253345E-2</v>
+        <v>2.7530766094265E-2</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
-        <v>0.76879039704524399</v>
+        <v>0.76934441366574302</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14">
-        <v>0.64253968253968197</v>
+        <v>0.78947368421052599</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
       <c r="H14">
-        <v>0.85121832575856504</v>
+        <v>0.85108623572032904</v>
       </c>
       <c r="I14">
         <v>0</v>
@@ -2692,25 +2644,25 @@
         <v>20</v>
       </c>
       <c r="B15">
-        <v>1.23697994630997E-2</v>
+        <v>1.2373290899468099E-2</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15">
-        <v>0.89307330195080903</v>
+        <v>0.88942118937537795</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
       <c r="F15">
-        <v>0.81355555555555503</v>
+        <v>0.875</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
       <c r="H15">
-        <v>0.97853867927567895</v>
+        <v>0.97870349811620305</v>
       </c>
       <c r="I15">
         <v>0</v>
@@ -2721,25 +2673,25 @@
         <v>21</v>
       </c>
       <c r="B16">
-        <v>7.89462553825079E-3</v>
+        <v>7.9539808780451204E-3</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16">
-        <v>0.92270819936510295</v>
+        <v>0.92143959548951304</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="F16">
-        <v>0.76772393071094303</v>
+        <v>0.939393939393939</v>
       </c>
       <c r="G16">
         <v>0</v>
       </c>
       <c r="H16">
-        <v>0.92659178732542002</v>
+        <v>0.92933967525314698</v>
       </c>
       <c r="I16">
         <v>0</v>
@@ -2750,25 +2702,25 @@
         <v>23</v>
       </c>
       <c r="B17">
-        <v>1.80267654095132E-3</v>
+        <v>1.7989952277666201E-3</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17">
-        <v>0.98809932978174897</v>
+        <v>0.98792747894827304</v>
       </c>
       <c r="E17">
         <v>0</v>
       </c>
       <c r="F17">
-        <v>0.92868200639939702</v>
+        <v>0.98913043478260798</v>
       </c>
       <c r="G17">
         <v>0</v>
       </c>
       <c r="H17">
-        <v>0.99311914164287496</v>
+        <v>0.99425083525449298</v>
       </c>
       <c r="I17">
         <v>0</v>
@@ -2779,25 +2731,25 @@
         <v>33</v>
       </c>
       <c r="B18">
-        <v>2.0708076293301601E-2</v>
+        <v>2.0704068522324499E-2</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18">
-        <v>0.928192351320693</v>
+        <v>0.92871900826446296</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="F18">
-        <v>0.75722181698510704</v>
+        <v>0.92156862745098</v>
       </c>
       <c r="G18">
         <v>0</v>
       </c>
       <c r="H18">
-        <v>0.87198133600296202</v>
+        <v>0.87178696397460698</v>
       </c>
       <c r="I18">
         <v>0</v>
@@ -2811,10 +2763,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2833,28 +2785,28 @@
         <v>5</v>
       </c>
       <c r="B1">
-        <v>2.53713094342988E-2</v>
+        <v>2.6824275480807801E-2</v>
       </c>
       <c r="C1">
-        <v>1.7375272644192301E-2</v>
+        <v>1.5764321153293199E-2</v>
       </c>
       <c r="D1">
-        <v>0.87333333333333296</v>
+        <v>0.9</v>
       </c>
       <c r="E1">
-        <v>0.122202018532155</v>
+        <v>0.13999999999999899</v>
       </c>
       <c r="F1">
-        <v>0.81111111111111101</v>
+        <v>0.97777777777777697</v>
       </c>
       <c r="G1">
-        <v>0.24570382652773301</v>
+        <v>3.8490017945975098E-2</v>
       </c>
       <c r="H1">
-        <v>0.93111934426067799</v>
+        <v>0.93282235593109597</v>
       </c>
       <c r="I1">
-        <v>0.109970224219978</v>
+        <v>0.111365836959813</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -2862,25 +2814,25 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>2.9408994506949299E-2</v>
+        <v>2.67132859574284E-2</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0.89523809523809506</v>
+        <v>0.92380952380952297</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0.98148148148148096</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>0.99647521864725797</v>
+        <v>0.99817812147912899</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -2891,28 +2843,28 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>2.0019547881525501E-2</v>
+        <v>2.31425664552002E-2</v>
       </c>
       <c r="C3">
-        <v>1.2512717333423001E-2</v>
+        <v>1.48067928919965E-2</v>
       </c>
       <c r="D3">
-        <v>0.871913589564416</v>
+        <v>0.865274395425222</v>
       </c>
       <c r="E3">
-        <v>0.131457001209317</v>
+        <v>0.13989032401443099</v>
       </c>
       <c r="F3">
-        <v>0.83613782051282004</v>
+        <v>0.86538461538461497</v>
       </c>
       <c r="G3">
-        <v>0.13032746953567201</v>
+        <v>0.125898215145899</v>
       </c>
       <c r="H3">
-        <v>0.95393688176893898</v>
+        <v>0.955497776164278</v>
       </c>
       <c r="I3">
-        <v>4.9147590797853802E-2</v>
+        <v>4.7503973139513801E-2</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -2920,28 +2872,28 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>2.0136482849471199E-2</v>
+        <v>2.3495008000735399E-2</v>
       </c>
       <c r="C4">
-        <v>1.44457556041197E-2</v>
+        <v>1.5599641359644799E-2</v>
       </c>
       <c r="D4">
-        <v>0.83568437030702003</v>
+        <v>0.83731617402802405</v>
       </c>
       <c r="E4">
-        <v>0.16564227359021699</v>
+        <v>0.15930951969790899</v>
       </c>
       <c r="F4">
-        <v>0.763348148148148</v>
+        <v>0.89688888888888796</v>
       </c>
       <c r="G4">
-        <v>0.184342232078445</v>
+        <v>0.10018090632335799</v>
       </c>
       <c r="H4">
-        <v>0.90187972150623097</v>
+        <v>0.89892634517564296</v>
       </c>
       <c r="I4">
-        <v>0.11985644698003201</v>
+        <v>0.10877767414772201</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -2949,28 +2901,28 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>1.43003974985117E-2</v>
+        <v>1.52676533670386E-2</v>
       </c>
       <c r="C5">
-        <v>9.01065114810801E-3</v>
+        <v>1.0100009553653E-2</v>
       </c>
       <c r="D5">
-        <v>0.88414902996042</v>
+        <v>0.88213455732289003</v>
       </c>
       <c r="E5">
-        <v>0.123133644282738</v>
+        <v>0.12055886020038099</v>
       </c>
       <c r="F5">
-        <v>0.82012903225806399</v>
+        <v>0.88593548387096699</v>
       </c>
       <c r="G5">
-        <v>0.133496893117409</v>
+        <v>0.109809142418529</v>
       </c>
       <c r="H5">
-        <v>0.93428774088857502</v>
+        <v>0.93257692002981196</v>
       </c>
       <c r="I5">
-        <v>7.7273945438372793E-2</v>
+        <v>7.4727421422603996E-2</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -2978,28 +2930,28 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <v>1.18473741967397E-2</v>
+        <v>1.2466162868590199E-2</v>
       </c>
       <c r="C6">
-        <v>5.4360729953337496E-3</v>
+        <v>5.3243719083130399E-3</v>
       </c>
       <c r="D6">
-        <v>0.90323468485580904</v>
+        <v>0.900917054311282</v>
       </c>
       <c r="E6">
-        <v>0.107781534508995</v>
+        <v>0.111169088979949</v>
       </c>
       <c r="F6">
-        <v>0.88606060606060599</v>
+        <v>0.89545454545454495</v>
       </c>
       <c r="G6">
-        <v>9.3037026435947301E-2</v>
+        <v>9.7528377981921294E-2</v>
       </c>
       <c r="H6">
-        <v>0.96611596082708195</v>
+        <v>0.96702327112215203</v>
       </c>
       <c r="I6">
-        <v>3.8001592007031897E-2</v>
+        <v>4.1124123150383697E-2</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -3007,28 +2959,28 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>2.55043635492594E-2</v>
+        <v>2.5521178840814399E-2</v>
       </c>
       <c r="C7">
-        <v>9.5578098285571504E-3</v>
+        <v>9.3684982629107204E-3</v>
       </c>
       <c r="D7">
-        <v>0.87694625063046105</v>
+        <v>0.87597908913698297</v>
       </c>
       <c r="E7">
-        <v>6.2404683853617499E-2</v>
+        <v>6.3668976897568993E-2</v>
       </c>
       <c r="F7">
-        <v>0.72322530864197498</v>
+        <v>0.81944444444444398</v>
       </c>
       <c r="G7">
-        <v>0.156445236963276</v>
+        <v>1.38888888888889E-2</v>
       </c>
       <c r="H7">
-        <v>0.87169876401981405</v>
+        <v>0.85686974580470099</v>
       </c>
       <c r="I7">
-        <v>0.104001109554501</v>
+        <v>0.11280351961559899</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -3036,28 +2988,28 @@
         <v>13</v>
       </c>
       <c r="B8">
-        <v>1.6451825624302301E-2</v>
+        <v>1.74735945613936E-2</v>
       </c>
       <c r="C8">
-        <v>1.25178536920993E-2</v>
+        <v>1.3769354769872099E-2</v>
       </c>
       <c r="D8">
-        <v>0.93794834756541301</v>
+        <v>0.93864199259050796</v>
       </c>
       <c r="E8">
-        <v>7.2185737160212801E-2</v>
+        <v>7.2386666072416894E-2</v>
       </c>
       <c r="F8">
-        <v>0.77343668236525298</v>
+        <v>0.95604395604395598</v>
       </c>
       <c r="G8">
-        <v>0.169953076549888</v>
+        <v>1.7944979800609301E-2</v>
       </c>
       <c r="H8">
-        <v>0.82259924189419298</v>
+        <v>0.82311710765713197</v>
       </c>
       <c r="I8">
-        <v>0.15784888156597801</v>
+        <v>0.158368480855583</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -3065,28 +3017,28 @@
         <v>14</v>
       </c>
       <c r="B9">
-        <v>2.3710710275535701E-2</v>
+        <v>2.3688014419403901E-2</v>
       </c>
       <c r="C9">
-        <v>3.0339835540402999E-2</v>
+        <v>3.0401135640758199E-2</v>
       </c>
       <c r="D9">
-        <v>0.94488139360968004</v>
+        <v>0.94617769342626301</v>
       </c>
       <c r="E9">
-        <v>2.6375727759949601E-2</v>
+        <v>2.5453420067175901E-2</v>
       </c>
       <c r="F9">
-        <v>0.908193634596695</v>
+        <v>0.88775510204081598</v>
       </c>
       <c r="G9">
-        <v>9.0097593455366998E-2</v>
+        <v>2.6346825484404202E-2</v>
       </c>
       <c r="H9">
-        <v>0.97985875488684604</v>
+        <v>0.97991904493109905</v>
       </c>
       <c r="I9">
-        <v>3.3038928126666797E-2</v>
+        <v>3.3054929158388202E-2</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -3094,28 +3046,28 @@
         <v>15</v>
       </c>
       <c r="B10">
-        <v>9.3539959846649506E-3</v>
+        <v>9.4252068614306406E-3</v>
       </c>
       <c r="C10">
-        <v>6.8018027041726603E-3</v>
+        <v>6.9030166424523098E-3</v>
       </c>
       <c r="D10">
-        <v>0.95368371763390103</v>
+        <v>0.95423071935802595</v>
       </c>
       <c r="E10">
-        <v>4.6066818023423002E-2</v>
+        <v>4.5016071477029101E-2</v>
       </c>
       <c r="F10">
-        <v>0.85109523809523802</v>
+        <v>0.97</v>
       </c>
       <c r="G10">
-        <v>0.108601569420764</v>
+        <v>3.8459935864047702E-2</v>
       </c>
       <c r="H10">
-        <v>0.93437459098126596</v>
+        <v>0.92863837335586996</v>
       </c>
       <c r="I10">
-        <v>7.6102795407862606E-2</v>
+        <v>8.0020544207184297E-2</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -3123,28 +3075,28 @@
         <v>16</v>
       </c>
       <c r="B11">
-        <v>1.1934534497139699E-2</v>
+        <v>1.18529249979586E-2</v>
       </c>
       <c r="C11">
-        <v>4.0604974111013298E-3</v>
+        <v>4.0371560923254304E-3</v>
       </c>
       <c r="D11">
-        <v>0.93704044117647001</v>
+        <v>0.93777573529411695</v>
       </c>
       <c r="E11">
-        <v>2.6906452887061501E-2</v>
+        <v>2.92461444424581E-2</v>
       </c>
       <c r="F11">
-        <v>0.88496093749999905</v>
+        <v>0.9375</v>
       </c>
       <c r="G11">
-        <v>9.9173830545879194E-3</v>
+        <v>7.7339804192278594E-2</v>
       </c>
       <c r="H11">
-        <v>0.99158615393371297</v>
+        <v>0.99057939970540398</v>
       </c>
       <c r="I11">
-        <v>2.4966373300413201E-3</v>
+        <v>4.8441530992826397E-3</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -3152,25 +3104,25 @@
         <v>17</v>
       </c>
       <c r="B12">
-        <v>6.60579708115325E-3</v>
+        <v>6.5932661005393897E-3</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12">
-        <v>0.97448096885813096</v>
+        <v>0.97390426758938797</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12">
-        <v>0.86362952588442699</v>
+        <v>0.99346405228758095</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
       <c r="H12">
-        <v>0.95071068150022697</v>
+        <v>0.95134008585220597</v>
       </c>
       <c r="I12">
         <v>0</v>
@@ -3181,25 +3133,25 @@
         <v>20</v>
       </c>
       <c r="B13">
-        <v>1.23697994630997E-2</v>
+        <v>1.2373290899468099E-2</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13">
-        <v>0.89307330195080903</v>
+        <v>0.88942118937537795</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="F13">
-        <v>0.81355555555555503</v>
+        <v>0.875</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13">
-        <v>0.97853867927567895</v>
+        <v>0.97870349811620305</v>
       </c>
       <c r="I13">
         <v>0</v>
@@ -3210,25 +3162,25 @@
         <v>21</v>
       </c>
       <c r="B14">
-        <v>7.89462553825079E-3</v>
+        <v>7.9539808780451204E-3</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
-        <v>0.92270819936510295</v>
+        <v>0.92143959548951304</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14">
-        <v>0.76772393071094303</v>
+        <v>0.939393939393939</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
       <c r="H14">
-        <v>0.92659178732542002</v>
+        <v>0.92933967525314698</v>
       </c>
       <c r="I14">
         <v>0</v>
@@ -3239,27 +3191,56 @@
         <v>23</v>
       </c>
       <c r="B15">
-        <v>1.80267654095132E-3</v>
+        <v>1.7989952277666201E-3</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15">
-        <v>0.98809932978174897</v>
+        <v>0.98792747894827304</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
       <c r="F15">
-        <v>0.92868200639939702</v>
+        <v>0.98913043478260798</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
       <c r="H15">
-        <v>0.99311914164287496</v>
+        <v>0.99425083525449298</v>
       </c>
       <c r="I15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16">
+        <v>33</v>
+      </c>
+      <c r="B16">
+        <v>2.0704068522324499E-2</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0.92871900826446296</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0.92156862745098</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0.87178696397460698</v>
+      </c>
+      <c r="I16">
         <v>0</v>
       </c>
     </row>

</xml_diff>